<commit_message>
[#14] update criteria list
</commit_message>
<xml_diff>
--- a/casus/criteria.xlsx
+++ b/casus/criteria.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvandenbrink\Documents\github\disgeo-imsor\casus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\git\Geonovum\disgeo-imsor\casus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBF3363-6CB2-4AFA-81DC-FD00B1BAD177}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8183CF-8443-4574-9E3A-4E39FF34A96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5400" windowWidth="38640" windowHeight="21240" xr2:uid="{54109986-20EF-4B6F-9356-2054A5B97786}"/>
+    <workbookView xWindow="29400" yWindow="2340" windowWidth="26010" windowHeight="15600" xr2:uid="{54109986-20EF-4B6F-9356-2054A5B97786}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Criteria" sheetId="1" r:id="rId1"/>
+    <sheet name="Voorbeeld" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>Is er een hoge mate van complexiteit in de oplossing?</t>
   </si>
@@ -45,9 +46,6 @@
     <t>Dekt de uitwerking de functionele use cases [1] af?</t>
   </si>
   <si>
-    <t>Is de uitwerking 'by convention' gemodelleerd die niet gestandaardiseerd is, oftewel: is er meer voor nodig dan MIM kennis om het model te begrijpen?</t>
-  </si>
-  <si>
     <t>Is de uitwerking standaard te serialiseren out of the box, dat wil zeggen zonder nieuwe encoding rules naar XML, RDF, en JSON?</t>
   </si>
   <si>
@@ -118,13 +116,41 @@
   </si>
   <si>
     <t>Is de uitwerking vooral geschikt voor registratie, of geschikt voor uitleveren?</t>
+  </si>
+  <si>
+    <t>Is de uitwerking 'by convention' gemodelleerd die niet gestandaardiseerd is, oftewel: is er meer voor nodig dan MIM kennis om het model te begrijpen?
+(Hierin kunnen eventueel beschreven MIM uitbreidingen meegeteld worden als MIM)</t>
+  </si>
+  <si>
+    <t>Opmerking</t>
+  </si>
+  <si>
+    <t>VoorbeeldAspect</t>
+  </si>
+  <si>
+    <t>Voldoet de uiwerking aan X?</t>
+  </si>
+  <si>
+    <t>Ja
+Omdat ….</t>
+  </si>
+  <si>
+    <t>Ja, deels
+Omdat …</t>
+  </si>
+  <si>
+    <t>Nee
+Omdat...</t>
+  </si>
+  <si>
+    <t>Mist er volgens jou een belangrijk criterium. Voeg deze, desgewenst, hieronder toe.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,16 +188,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -203,13 +265,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -225,7 +305,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,10 +312,28 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Goed" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Invoer" xfId="5" builtinId="20"/>
     <cellStyle name="Kop 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Neutraal" xfId="4" builtinId="28"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,11 +646,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75C2D25E-2EFE-4570-A07E-3A7ACD9EFA21}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -563,167 +658,385 @@
     <col min="5" max="5" width="40.7109375" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
     <col min="7" max="7" width="47.7109375" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="35.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="H1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="35.25" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>15</v>
+      <c r="B2" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="69" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:8" ht="120.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" ht="69" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="69" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>4</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>5</v>
-      </c>
-      <c r="B6" s="9" t="s">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
-        <v>8</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -736,4 +1049,72 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CB535E-71B9-41EC-94BD-4B5B03081AE3}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>